<commit_message>
rev 2 changes, see revision_log
</commit_message>
<xml_diff>
--- a/VCO/Assembly/smd_bom.xlsx
+++ b/VCO/Assembly/smd_bom.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
   <si>
     <t>Comment</t>
   </si>
@@ -151,10 +151,10 @@
     <t>C10,C9,C8,C6,C5,C4,C3</t>
   </si>
   <si>
-    <t>C_0402</t>
-  </si>
-  <si>
-    <t>C1525</t>
+    <t>C_0603</t>
+  </si>
+  <si>
+    <t>C14663</t>
   </si>
   <si>
     <t>3.3nF*</t>
@@ -191,6 +191,18 @@
   </si>
   <si>
     <t>C8655</t>
+  </si>
+  <si>
+    <t>MMBFJ112</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>C258195</t>
   </si>
   <si>
     <t>SCH</t>
@@ -254,6 +266,7 @@
     <font>
       <b/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
     </font>
     <font/>
     <font>
@@ -286,7 +299,7 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -767,13 +780,13 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -781,13 +794,13 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -809,17 +822,31 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rev 3, see revision log
</commit_message>
<xml_diff>
--- a/VCO/Assembly/smd_bom.xlsx
+++ b/VCO/Assembly/smd_bom.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="89">
   <si>
     <t>Comment</t>
   </si>
@@ -37,10 +37,19 @@
     <t>C17407</t>
   </si>
   <si>
+    <t>91K</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>C137484</t>
+  </si>
+  <si>
     <t>56K</t>
   </si>
   <si>
-    <t>R7,R16,R1</t>
+    <t>R7,R16</t>
   </si>
   <si>
     <t>C17756</t>
@@ -145,6 +154,27 @@
     <t>C17629</t>
   </si>
   <si>
+    <t>330pF</t>
+  </si>
+  <si>
+    <t>C11,C12</t>
+  </si>
+  <si>
+    <t>C_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>C51207</t>
+  </si>
+  <si>
+    <t>4.7pF</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C1820</t>
+  </si>
+  <si>
     <t>100nF</t>
   </si>
   <si>
@@ -161,9 +191,6 @@
   </si>
   <si>
     <t>C7</t>
-  </si>
-  <si>
-    <t>C_0805_2012Metric</t>
   </si>
   <si>
     <t>C76473</t>
@@ -731,122 +758,164 @@
         <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="2" t="s">
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="2" t="s">
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="3" t="s">
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="3" t="s">
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>79</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>